<commit_message>
Allow for sequential project loading.
</commit_message>
<xml_diff>
--- a/Test/2018.49 Testing 49/Project_Information.xlsx
+++ b/Test/2018.49 Testing 49/Project_Information.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Fast/tim/Documents/code/dev/PSW/Test/2018.49 Testing 49/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728D2D5B-E92D-EB45-A287-2FF072E71480}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" windowHeight="16940" windowWidth="27640" xWindow="2620" yWindow="480"/>
+    <workbookView xWindow="2620" yWindow="480" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Project Information</t>
   </si>
@@ -46,18 +52,12 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Revit</t>
-  </si>
-  <si>
     <t>Revit or CAD or Other</t>
   </si>
   <si>
     <t>Scope</t>
   </si>
   <si>
-    <t>Scoep for 49</t>
-  </si>
-  <si>
     <t>Description of the project</t>
   </si>
   <si>
@@ -95,56 +95,58 @@
   </si>
   <si>
     <t>Scope for 49</t>
+  </si>
+  <si>
+    <t>Default</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF3F3F76"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <i val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="10"/>
-      <sz val="12"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -272,66 +274,75 @@
     </border>
   </borders>
   <cellStyleXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="3" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="9" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="20" name="Input" xfId="1"/>
-    <cellStyle builtinId="53" name="Explanatory Text" xfId="2"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="3"/>
+    <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -631,73 +642,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="17.1640625"/>
-    <col customWidth="1" max="3" min="3" width="27"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="31.33203125"/>
+    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="9" t="n"/>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="9"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="n"/>
-      <c r="E1" s="9" t="n"/>
-    </row>
-    <row customHeight="1" ht="17" r="2" spans="1:5" thickBot="1">
-      <c r="A2" s="9" t="n"/>
-      <c r="B2" s="9" t="n"/>
-      <c r="C2" s="9" t="n"/>
-      <c r="D2" s="2" t="n"/>
-      <c r="E2" s="9" t="n"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="9" t="n"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="9"/>
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="n"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="9" t="n"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="9" t="n"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="9"/>
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7" t="n"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="9" t="n"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="9" t="n"/>
-      <c r="B5" s="6" t="n"/>
-      <c r="C5" s="9" t="n"/>
-      <c r="D5" s="8" t="n"/>
-      <c r="E5" s="9" t="n"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="9" t="n"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="9"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="9"/>
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
@@ -707,207 +714,207 @@
       <c r="D6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="9" t="n"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="9" t="n"/>
-      <c r="B7" s="6" t="n"/>
-      <c r="C7" s="9" t="n"/>
-      <c r="D7" s="8" t="n"/>
-      <c r="E7" s="9" t="n"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="9" t="n"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="9"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="9"/>
       <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="9"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="9" t="n"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="9" t="n"/>
-      <c r="B9" s="6" t="n"/>
-      <c r="C9" s="9" t="n"/>
-      <c r="D9" s="8" t="n"/>
-      <c r="E9" s="9" t="n"/>
-    </row>
-    <row customHeight="1" ht="49" r="10" spans="1:5" thickBot="1">
-      <c r="A10" s="9" t="n"/>
-      <c r="B10" s="10" t="s">
+      <c r="C10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="15" t="s">
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="9"/>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="9" t="n"/>
-    </row>
-    <row customHeight="1" ht="17" r="11" spans="1:5" thickBot="1">
-      <c r="A11" s="9" t="n"/>
-      <c r="B11" s="9" t="n"/>
-      <c r="C11" s="9" t="n"/>
-      <c r="D11" s="2" t="n"/>
-      <c r="E11" s="9" t="n"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="9" t="n"/>
-      <c r="B12" s="3" t="s">
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="9"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="12" t="s"/>
-      <c r="D12" s="5" t="s">
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="9"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="9" t="n"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="9" t="n"/>
-      <c r="B13" s="6" t="n"/>
-      <c r="C13" s="7" t="s"/>
-      <c r="D13" s="8" t="s">
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="9"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="9" t="n"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="9" t="n"/>
-      <c r="B14" s="6" t="n"/>
-      <c r="C14" s="7" t="s"/>
-      <c r="D14" s="8" t="s">
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="9"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="9"/>
+      <c r="B17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="9" t="n"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="9" t="n"/>
-      <c r="B15" s="6" t="n"/>
-      <c r="C15" s="13" t="s"/>
-      <c r="D15" s="8" t="s">
+      <c r="C17" s="7"/>
+      <c r="D17" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="9" t="n"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="9" t="n"/>
-      <c r="B16" s="6" t="n"/>
-      <c r="C16" s="9" t="n"/>
-      <c r="D16" s="8" t="n"/>
-      <c r="E16" s="9" t="n"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="9" t="n"/>
-      <c r="B17" s="6" t="s">
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:5" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="7" t="s"/>
-      <c r="D17" s="8" t="s">
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="9"/>
+      <c r="B20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="9" t="n"/>
-    </row>
-    <row customHeight="1" ht="17" r="18" spans="1:5" thickBot="1">
-      <c r="A18" s="9" t="n"/>
-      <c r="B18" s="10" t="n"/>
-      <c r="C18" s="14" t="s"/>
-      <c r="D18" s="15" t="s">
+      <c r="C20" s="12"/>
+      <c r="D20" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="9" t="n"/>
-    </row>
-    <row customHeight="1" ht="17" r="19" spans="1:5" thickBot="1">
-      <c r="A19" s="9" t="n"/>
-      <c r="B19" s="9" t="n"/>
-      <c r="C19" s="9" t="n"/>
-      <c r="D19" s="2" t="n"/>
-      <c r="E19" s="9" t="n"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="9" t="n"/>
-      <c r="B20" s="3" t="s">
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="9"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="9"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="9"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="9"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="9"/>
+      <c r="B25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="12" t="s"/>
-      <c r="D20" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="9" t="n"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="9" t="n"/>
-      <c r="B21" s="6" t="n"/>
-      <c r="C21" s="7" t="s"/>
-      <c r="D21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="9" t="n"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="9" t="n"/>
-      <c r="B22" s="6" t="n"/>
-      <c r="C22" s="7" t="s"/>
-      <c r="D22" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="9" t="n"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="9" t="n"/>
-      <c r="B23" s="6" t="n"/>
-      <c r="C23" s="13" t="s"/>
-      <c r="D23" s="8" t="s">
+      <c r="C25" s="7"/>
+      <c r="D25" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="9" t="n"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="9" t="n"/>
-      <c r="B24" s="6" t="n"/>
-      <c r="C24" s="9" t="n"/>
-      <c r="D24" s="8" t="n"/>
-      <c r="E24" s="9" t="n"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="9" t="n"/>
-      <c r="B25" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="7" t="s"/>
-      <c r="D25" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="9" t="n"/>
-    </row>
-    <row customHeight="1" ht="17" r="26" spans="1:5" thickBot="1">
-      <c r="A26" s="9" t="n"/>
-      <c r="B26" s="10" t="n"/>
-      <c r="C26" s="14" t="s"/>
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="1:5" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="14"/>
       <c r="D26" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="9" t="n"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="9" t="n"/>
-      <c r="B27" s="9" t="n"/>
-      <c r="C27" s="9" t="n"/>
-      <c r="D27" s="2" t="n"/>
-      <c r="E27" s="9" t="n"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="9" t="n"/>
-      <c r="B28" s="9" t="n"/>
-      <c r="C28" s="9" t="n"/>
-      <c r="D28" s="2" t="n"/>
-      <c r="E28" s="9" t="n"/>
+        <v>20</v>
+      </c>
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="9"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="9"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>